<commit_message>
use the new roscop object, attributes variable is now dynamic
</commit_message>
<xml_diff>
--- a/roscop/code_roscop_all.xlsx
+++ b/roscop/code_roscop_all.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="code_roscop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -2448,7 +2448,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0E+00"/>
+    <numFmt numFmtId="164" formatCode="0E+00"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -2948,7 +2948,7 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2961,7 +2961,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3301,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="A291" sqref="A291:G291"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>